<commit_message>
support pageable in each directive
</commit_message>
<xml_diff>
--- a/excel/src/test/resources/multisheet_markup_template.xlsx
+++ b/excel/src/test/resources/multisheet_markup_template.xlsx
@@ -116,7 +116,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+  <si>
+    <t>ddddd</t>
+  </si>
   <si>
     <t>Department:</t>
   </si>
@@ -195,11 +198,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_)@"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;&quot;р.&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_р_._-;\-* #,##0_р_._-;_-* &quot;-&quot;_р_._-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;&quot;р.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_р_._-;\-* #,##0_р_._-;_-* &quot;-&quot;_р_._-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_)@"/>
     <numFmt numFmtId="181" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="33">
@@ -207,7 +210,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -216,27 +218,23 @@
       <sz val="16"/>
       <color theme="3"/>
       <name val="Cambria"/>
-      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="3"/>
       <name val="Cambria"/>
-      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
-      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="0"/>
     </font>
     <font>
@@ -244,7 +242,6 @@
       <sz val="10.5"/>
       <color theme="2" tint="-0.499984740745262"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -252,7 +249,6 @@
       <sz val="11"/>
       <color theme="3" tint="-0.499984740745262"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -260,7 +256,6 @@
       <sz val="11"/>
       <color rgb="FF0070C0"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -268,7 +263,6 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -276,7 +270,6 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -285,7 +278,6 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -293,7 +285,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -301,7 +292,6 @@
       <b/>
       <sz val="10"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -309,7 +299,6 @@
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -317,7 +306,6 @@
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -325,7 +313,6 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -334,7 +321,6 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -343,7 +329,6 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -352,7 +337,6 @@
       <sz val="11"/>
       <color theme="3"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -360,7 +344,6 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -369,7 +352,6 @@
       <sz val="18"/>
       <color theme="3"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -378,7 +360,6 @@
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -387,7 +368,6 @@
       <sz val="15"/>
       <color theme="3"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -396,7 +376,6 @@
       <sz val="13"/>
       <color theme="3"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -405,7 +384,6 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -414,7 +392,6 @@
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -423,7 +400,6 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -431,7 +407,6 @@
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -440,7 +415,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -448,7 +422,6 @@
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -456,7 +429,6 @@
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="方正舒体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -837,14 +809,14 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -898,17 +870,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="5" fillId="2" borderId="1" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="1" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="5" fillId="2" borderId="2" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="2" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="2" borderId="0" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="0" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1258,7 +1230,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88333333333333" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -1270,14 +1242,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" ht="37.5" customHeight="1" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1286,10 +1260,10 @@
     </row>
     <row r="3" ht="37.5" customHeight="1" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -1298,10 +1272,10 @@
     </row>
     <row r="4" ht="37.5" customHeight="1" spans="1:6">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1310,10 +1284,10 @@
     </row>
     <row r="5" ht="37.5" customHeight="1" spans="1:6">
       <c r="A5" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -1323,76 +1297,76 @@
     <row r="6" ht="13.95"/>
     <row r="7" spans="1:6">
       <c r="A7" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" ht="24" spans="1:6">
       <c r="A9" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>